<commit_message>
begin working on debug, implement custom services, fix ServiceNotificationType.Shutdown not actually working
</commit_message>
<xml_diff>
--- a/Lightning.Documentation/M4Schedule.xlsx
+++ b/Lightning.Documentation/M4Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FiercePC\Lightning\Lightning\Lightning.Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0134D62-9A8D-4CBA-BB02-C2B757CA50C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2846B17F-30B6-4290-9353-DD4DE7C65C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{454DAF17-9AC5-48F2-BE3E-2A10673E522A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
   <si>
     <t>Feature</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Event: OnAnimationStopped</t>
   </si>
   <si>
-    <t>OnTrigger animations</t>
-  </si>
-  <si>
     <t>Bugfix for nonrelative paths in DDMS</t>
   </si>
   <si>
@@ -135,9 +132,6 @@
     <t>Event: OnObjectCreated</t>
   </si>
   <si>
-    <t>Fix Win32 Dialog File Names (Lightning.Core.NativeInterop)</t>
-  </si>
-  <si>
     <t>Event: OnCollisionStart</t>
   </si>
   <si>
@@ -166,6 +160,30 @@
   </si>
   <si>
     <t>Physics - Only Stop in one direction on Collision in that direction</t>
+  </si>
+  <si>
+    <t>OnEvent / FromScript animations</t>
+  </si>
+  <si>
+    <t>Aug 20, 2021</t>
+  </si>
+  <si>
+    <t>Aug 19, 2021</t>
+  </si>
+  <si>
+    <t>DDMS Objects know when fully loaded from XML</t>
+  </si>
+  <si>
+    <t>Welcome Document</t>
+  </si>
+  <si>
+    <t>External - Documentation</t>
+  </si>
+  <si>
+    <t>Lua Documentation</t>
+  </si>
+  <si>
+    <t>Fix Win32 Dialog File Names (Lightning.Core.NativeInterop.Win32)</t>
   </si>
 </sst>
 </file>
@@ -194,7 +212,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,6 +243,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -238,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -246,6 +270,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCF3E34E-818E-4A9E-84CD-2F8F367ADE0E}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -582,7 +607,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -625,7 +650,7 @@
     </row>
     <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>7</v>
@@ -633,10 +658,16 @@
     </row>
     <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>0</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -646,6 +677,12 @@
       <c r="B9" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="C9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -681,7 +718,7 @@
     </row>
     <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>0</v>
@@ -689,7 +726,7 @@
     </row>
     <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>0</v>
@@ -697,7 +734,7 @@
     </row>
     <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>0</v>
@@ -705,7 +742,7 @@
     </row>
     <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>7</v>
@@ -713,7 +750,7 @@
     </row>
     <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>5</v>
@@ -729,7 +766,7 @@
     </row>
     <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>0</v>
@@ -737,7 +774,7 @@
     </row>
     <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>0</v>
@@ -745,7 +782,7 @@
     </row>
     <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>7</v>
@@ -753,61 +790,67 @@
     </row>
     <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>0</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>0</v>
+    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>5</v>
+        <v>21</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>0</v>
+        <v>52</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>0</v>
@@ -815,7 +858,7 @@
     </row>
     <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>0</v>
@@ -823,7 +866,7 @@
     </row>
     <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>0</v>
@@ -831,7 +874,7 @@
     </row>
     <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>0</v>
@@ -839,7 +882,7 @@
     </row>
     <row r="35" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>0</v>
@@ -847,7 +890,7 @@
     </row>
     <row r="36" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>0</v>
@@ -855,7 +898,7 @@
     </row>
     <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>0</v>
@@ -863,7 +906,7 @@
     </row>
     <row r="38" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>0</v>
@@ -871,7 +914,7 @@
     </row>
     <row r="39" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>0</v>
@@ -879,7 +922,7 @@
     </row>
     <row r="40" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>0</v>
@@ -887,10 +930,34 @@
     </row>
     <row r="41" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B41" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
oof i barely did anything stop getting distracted by game source code leaks
</commit_message>
<xml_diff>
--- a/Lightning.Documentation/M4Schedule.xlsx
+++ b/Lightning.Documentation/M4Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FiercePC\Lightning\Lightning\Lightning.Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2846B17F-30B6-4290-9353-DD4DE7C65C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78C9037-4208-4F4B-95D6-D84B8E3F7BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{454DAF17-9AC5-48F2-BE3E-2A10673E522A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="57">
   <si>
     <t>Feature</t>
   </si>
@@ -69,9 +69,6 @@
     <t>IGDService (In-Game Debugging Service)</t>
   </si>
   <si>
-    <t>Event: OnAnimationFrameChanged</t>
-  </si>
-  <si>
     <t>Event: OnAnimationStarted</t>
   </si>
   <si>
@@ -156,15 +153,9 @@
     <t>Event: OnLevelLoaded</t>
   </si>
   <si>
-    <t>August 18, 2021 (Updated August 19, 2021)</t>
-  </si>
-  <si>
     <t>Physics - Only Stop in one direction on Collision in that direction</t>
   </si>
   <si>
-    <t>OnEvent / FromScript animations</t>
-  </si>
-  <si>
     <t>Aug 20, 2021</t>
   </si>
   <si>
@@ -184,6 +175,27 @@
   </si>
   <si>
     <t>Fix Win32 Dialog File Names (Lightning.Core.NativeInterop.Win32)</t>
+  </si>
+  <si>
+    <t>August 18, 2021 (Updated August 21, 2021)</t>
+  </si>
+  <si>
+    <t>Nested menus</t>
+  </si>
+  <si>
+    <t>Event: OnAnimationUpdated</t>
+  </si>
+  <si>
+    <t>Aug 21, 2021</t>
+  </si>
+  <si>
+    <t>Bugfix for service killing</t>
+  </si>
+  <si>
+    <t>Custom animations</t>
+  </si>
+  <si>
+    <t>Partially? Complete</t>
   </si>
 </sst>
 </file>
@@ -212,7 +224,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -249,6 +261,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -262,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -271,6 +289,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCF3E34E-818E-4A9E-84CD-2F8F367ADE0E}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -607,7 +626,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -650,7 +669,7 @@
     </row>
     <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>7</v>
@@ -658,16 +677,16 @@
     </row>
     <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -678,10 +697,10 @@
         <v>0</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -694,15 +713,21 @@
     </row>
     <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>0</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>0</v>
@@ -710,7 +735,7 @@
     </row>
     <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>0</v>
@@ -718,7 +743,7 @@
     </row>
     <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>0</v>
@@ -726,7 +751,7 @@
     </row>
     <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>0</v>
@@ -734,23 +759,32 @@
     </row>
     <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>0</v>
       </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
     </row>
     <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>7</v>
       </c>
+      <c r="C18" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>5</v>
@@ -766,7 +800,7 @@
     </row>
     <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>0</v>
@@ -774,7 +808,7 @@
     </row>
     <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>0</v>
@@ -782,7 +816,7 @@
     </row>
     <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>7</v>
@@ -790,35 +824,35 @@
     </row>
     <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C24" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>7</v>
@@ -826,31 +860,37 @@
     </row>
     <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>7</v>
       </c>
     </row>
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B30" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>5</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>0</v>
@@ -858,15 +898,15 @@
     </row>
     <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>0</v>
+        <v>49</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>0</v>
@@ -874,7 +914,7 @@
     </row>
     <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>0</v>
@@ -882,7 +922,7 @@
     </row>
     <row r="35" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>0</v>
@@ -890,7 +930,7 @@
     </row>
     <row r="36" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>0</v>
@@ -898,7 +938,7 @@
     </row>
     <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>0</v>
@@ -906,7 +946,7 @@
     </row>
     <row r="38" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>0</v>
@@ -914,7 +954,7 @@
     </row>
     <row r="39" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>0</v>
@@ -922,7 +962,7 @@
     </row>
     <row r="40" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>0</v>
@@ -930,7 +970,7 @@
     </row>
     <row r="41" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>0</v>
@@ -938,26 +978,42 @@
     </row>
     <row r="42" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>7</v>
+        <v>31</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>50</v>
+        <v>38</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish up basic igd stuff
</commit_message>
<xml_diff>
--- a/Lightning.Documentation/M4Schedule.xlsx
+++ b/Lightning.Documentation/M4Schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FiercePC\Lightning\Lightning\Lightning.Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78C9037-4208-4F4B-95D6-D84B8E3F7BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68682297-04A4-4013-A984-B08329DC23B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{454DAF17-9AC5-48F2-BE3E-2A10673E522A}"/>
   </bookViews>
@@ -84,9 +84,6 @@
     <t>DebugMode GameSetting (IGDService terminates if not set)</t>
   </si>
   <si>
-    <t>BaseException handling added to error messages</t>
-  </si>
-  <si>
     <t>Polaris: Insert Object</t>
   </si>
   <si>
@@ -196,6 +193,9 @@
   </si>
   <si>
     <t>Partially? Complete</t>
+  </si>
+  <si>
+    <t>BaseException handling added to error messages where required</t>
   </si>
 </sst>
 </file>
@@ -606,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCF3E34E-818E-4A9E-84CD-2F8F367ADE0E}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -626,7 +626,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -669,7 +669,7 @@
     </row>
     <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>7</v>
@@ -677,16 +677,16 @@
     </row>
     <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -697,10 +697,10 @@
         <v>0</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -713,16 +713,16 @@
     </row>
     <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -743,7 +743,7 @@
     </row>
     <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>0</v>
@@ -751,7 +751,7 @@
     </row>
     <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>0</v>
@@ -759,7 +759,7 @@
     </row>
     <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>0</v>
@@ -770,16 +770,16 @@
     </row>
     <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -816,7 +816,7 @@
     </row>
     <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>7</v>
@@ -824,35 +824,35 @@
     </row>
     <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C24" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>7</v>
@@ -860,7 +860,7 @@
     </row>
     <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>7</v>
@@ -868,7 +868,7 @@
     </row>
     <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>7</v>
@@ -876,21 +876,21 @@
     </row>
     <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>0</v>
@@ -898,7 +898,7 @@
     </row>
     <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>5</v>
@@ -906,7 +906,7 @@
     </row>
     <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>0</v>
@@ -914,7 +914,7 @@
     </row>
     <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>0</v>
@@ -922,7 +922,7 @@
     </row>
     <row r="35" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>0</v>
@@ -930,7 +930,7 @@
     </row>
     <row r="36" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>0</v>
@@ -938,7 +938,7 @@
     </row>
     <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>0</v>
@@ -946,7 +946,7 @@
     </row>
     <row r="38" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>0</v>
@@ -954,7 +954,7 @@
     </row>
     <row r="39" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>0</v>
@@ -962,7 +962,7 @@
     </row>
     <row r="40" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>0</v>
@@ -970,7 +970,7 @@
     </row>
     <row r="41" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>0</v>
@@ -978,7 +978,7 @@
     </row>
     <row r="42" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>0</v>
@@ -986,7 +986,7 @@
     </row>
     <row r="43" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>0</v>
@@ -994,7 +994,7 @@
     </row>
     <row r="44" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>7</v>
@@ -1002,18 +1002,18 @@
     </row>
     <row r="45" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>